<commit_message>
Update data dictionary, DOCX, and PDF files
</commit_message>
<xml_diff>
--- a/public/export/COVID AMP data dictionary 120920.xlsx
+++ b/public/export/COVID AMP data dictionary 120920.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mikevanmaele/Documents/GitHub/covid-npi-policy/public/export/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A5292F29-4D15-5549-A57F-A92B12539150}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D60024E2-E282-5E4B-BB16-BCEC3A7764C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="520" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="672">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="673">
   <si>
     <t>Unique ID</t>
   </si>
@@ -3809,6 +3809,9 @@
   </si>
   <si>
     <t>specific social distancing measures or guidelines included in the plan</t>
+  </si>
+  <si>
+    <t>Data dictionary: definitions of each category/column available in the COVID-AMP Court challenge database</t>
   </si>
 </sst>
 </file>
@@ -4951,48 +4954,45 @@
     <xf numFmtId="0" fontId="15" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -5018,6 +5018,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -7223,66 +7226,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="149"/>
-      <c r="B1" s="149"/>
-      <c r="C1" s="149"/>
-      <c r="D1" s="149"/>
+      <c r="A1" s="146"/>
+      <c r="B1" s="146"/>
+      <c r="C1" s="146"/>
+      <c r="D1" s="146"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="149"/>
-      <c r="B2" s="149"/>
-      <c r="C2" s="149"/>
-      <c r="D2" s="149"/>
+      <c r="A2" s="146"/>
+      <c r="B2" s="146"/>
+      <c r="C2" s="146"/>
+      <c r="D2" s="146"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="149"/>
-      <c r="B3" s="149"/>
-      <c r="C3" s="149"/>
-      <c r="D3" s="149"/>
+      <c r="A3" s="146"/>
+      <c r="B3" s="146"/>
+      <c r="C3" s="146"/>
+      <c r="D3" s="146"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="149"/>
-      <c r="B4" s="149"/>
-      <c r="C4" s="149"/>
-      <c r="D4" s="149"/>
+      <c r="A4" s="146"/>
+      <c r="B4" s="146"/>
+      <c r="C4" s="146"/>
+      <c r="D4" s="146"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="149"/>
-      <c r="B5" s="149"/>
-      <c r="C5" s="149"/>
-      <c r="D5" s="149"/>
+      <c r="A5" s="146"/>
+      <c r="B5" s="146"/>
+      <c r="C5" s="146"/>
+      <c r="D5" s="146"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="149"/>
-      <c r="B6" s="149"/>
-      <c r="C6" s="149"/>
-      <c r="D6" s="149"/>
+      <c r="A6" s="146"/>
+      <c r="B6" s="146"/>
+      <c r="C6" s="146"/>
+      <c r="D6" s="146"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="149"/>
-      <c r="B7" s="149"/>
-      <c r="C7" s="149"/>
-      <c r="D7" s="149"/>
+      <c r="A7" s="146"/>
+      <c r="B7" s="146"/>
+      <c r="C7" s="146"/>
+      <c r="D7" s="146"/>
     </row>
     <row r="8" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="150" t="s">
+      <c r="A8" s="147" t="s">
         <v>259</v>
       </c>
-      <c r="B8" s="150"/>
-      <c r="C8" s="150"/>
-      <c r="D8" s="150"/>
+      <c r="B8" s="147"/>
+      <c r="C8" s="147"/>
+      <c r="D8" s="147"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="150"/>
-      <c r="B9" s="150"/>
-      <c r="C9" s="150"/>
-      <c r="D9" s="150"/>
+      <c r="A9" s="147"/>
+      <c r="B9" s="147"/>
+      <c r="C9" s="147"/>
+      <c r="D9" s="147"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="151"/>
-      <c r="B10" s="151"/>
-      <c r="C10" s="151"/>
-      <c r="D10" s="151"/>
+      <c r="A10" s="148"/>
+      <c r="B10" s="148"/>
+      <c r="C10" s="148"/>
+      <c r="D10" s="148"/>
     </row>
     <row r="11" spans="1:4" s="2" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="32" t="s">
@@ -7311,21 +7314,21 @@
       <c r="D12" s="32"/>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="154" t="s">
+      <c r="A13" s="153" t="s">
         <v>513</v>
       </c>
-      <c r="B13" s="155"/>
-      <c r="C13" s="155"/>
-      <c r="D13" s="156"/>
+      <c r="B13" s="154"/>
+      <c r="C13" s="154"/>
+      <c r="D13" s="155"/>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="157"/>
-      <c r="B14" s="158"/>
-      <c r="C14" s="158"/>
-      <c r="D14" s="159"/>
+      <c r="A14" s="156"/>
+      <c r="B14" s="157"/>
+      <c r="C14" s="157"/>
+      <c r="D14" s="158"/>
     </row>
     <row r="15" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A15" s="139" t="s">
+      <c r="A15" s="149" t="s">
         <v>248</v>
       </c>
       <c r="B15" s="57" t="s">
@@ -7339,7 +7342,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A16" s="139"/>
+      <c r="A16" s="149"/>
       <c r="B16" s="57" t="s">
         <v>84</v>
       </c>
@@ -7351,7 +7354,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A17" s="139"/>
+      <c r="A17" s="149"/>
       <c r="B17" s="57" t="s">
         <v>167</v>
       </c>
@@ -7361,7 +7364,7 @@
       <c r="D17" s="30"/>
     </row>
     <row r="18" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A18" s="139"/>
+      <c r="A18" s="149"/>
       <c r="B18" s="57" t="s">
         <v>89</v>
       </c>
@@ -7371,7 +7374,7 @@
       <c r="D18" s="30"/>
     </row>
     <row r="19" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A19" s="139"/>
+      <c r="A19" s="149"/>
       <c r="B19" s="57" t="s">
         <v>93</v>
       </c>
@@ -7381,7 +7384,7 @@
       <c r="D19" s="30"/>
     </row>
     <row r="20" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A20" s="139"/>
+      <c r="A20" s="149"/>
       <c r="B20" s="57" t="s">
         <v>62</v>
       </c>
@@ -7391,7 +7394,7 @@
       <c r="D20" s="30"/>
     </row>
     <row r="21" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A21" s="139"/>
+      <c r="A21" s="149"/>
       <c r="B21" s="57" t="s">
         <v>70</v>
       </c>
@@ -7403,7 +7406,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A22" s="139"/>
+      <c r="A22" s="149"/>
       <c r="B22" s="57" t="s">
         <v>456</v>
       </c>
@@ -7413,7 +7416,7 @@
       <c r="D22" s="30"/>
     </row>
     <row r="23" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A23" s="139"/>
+      <c r="A23" s="149"/>
       <c r="B23" s="57" t="s">
         <v>90</v>
       </c>
@@ -7423,7 +7426,7 @@
       <c r="D23" s="30"/>
     </row>
     <row r="24" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A24" s="139"/>
+      <c r="A24" s="149"/>
       <c r="B24" s="57" t="s">
         <v>74</v>
       </c>
@@ -7433,7 +7436,7 @@
       <c r="D24" s="30"/>
     </row>
     <row r="25" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A25" s="139"/>
+      <c r="A25" s="149"/>
       <c r="B25" s="57" t="s">
         <v>72</v>
       </c>
@@ -7443,7 +7446,7 @@
       <c r="D25" s="30"/>
     </row>
     <row r="26" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A26" s="139"/>
+      <c r="A26" s="149"/>
       <c r="B26" s="57" t="s">
         <v>43</v>
       </c>
@@ -7453,7 +7456,7 @@
       <c r="D26" s="30"/>
     </row>
     <row r="27" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A27" s="139"/>
+      <c r="A27" s="149"/>
       <c r="B27" s="57" t="s">
         <v>46</v>
       </c>
@@ -7463,7 +7466,7 @@
       <c r="D27" s="30"/>
     </row>
     <row r="28" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A28" s="139"/>
+      <c r="A28" s="149"/>
       <c r="B28" s="57" t="s">
         <v>75</v>
       </c>
@@ -7473,7 +7476,7 @@
       <c r="D28" s="30"/>
     </row>
     <row r="29" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A29" s="139"/>
+      <c r="A29" s="149"/>
       <c r="B29" s="57" t="s">
         <v>71</v>
       </c>
@@ -7483,7 +7486,7 @@
       <c r="D29" s="30"/>
     </row>
     <row r="30" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A30" s="139"/>
+      <c r="A30" s="149"/>
       <c r="B30" s="57" t="s">
         <v>88</v>
       </c>
@@ -7493,7 +7496,7 @@
       <c r="D30" s="30"/>
     </row>
     <row r="31" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A31" s="139"/>
+      <c r="A31" s="149"/>
       <c r="B31" s="57" t="s">
         <v>509</v>
       </c>
@@ -7503,7 +7506,7 @@
       <c r="D31" s="30"/>
     </row>
     <row r="32" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A32" s="139"/>
+      <c r="A32" s="149"/>
       <c r="B32" s="57" t="s">
         <v>42</v>
       </c>
@@ -7513,7 +7516,7 @@
       <c r="D32" s="30"/>
     </row>
     <row r="33" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="140" t="s">
+      <c r="A33" s="151" t="s">
         <v>169</v>
       </c>
       <c r="B33" s="31" t="s">
@@ -7525,7 +7528,7 @@
       <c r="D33" s="31"/>
     </row>
     <row r="34" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A34" s="140"/>
+      <c r="A34" s="151"/>
       <c r="B34" s="31" t="s">
         <v>170</v>
       </c>
@@ -7535,7 +7538,7 @@
       <c r="D34" s="31"/>
     </row>
     <row r="35" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="139" t="s">
+      <c r="A35" s="149" t="s">
         <v>242</v>
       </c>
       <c r="B35" s="57" t="s">
@@ -7547,7 +7550,7 @@
       <c r="D35" s="30"/>
     </row>
     <row r="36" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="139"/>
+      <c r="A36" s="149"/>
       <c r="B36" s="57" t="s">
         <v>65</v>
       </c>
@@ -7557,7 +7560,7 @@
       <c r="D36" s="30"/>
     </row>
     <row r="37" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="139"/>
+      <c r="A37" s="149"/>
       <c r="B37" s="57" t="s">
         <v>92</v>
       </c>
@@ -7567,7 +7570,7 @@
       <c r="D37" s="30"/>
     </row>
     <row r="38" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="139"/>
+      <c r="A38" s="149"/>
       <c r="B38" s="57" t="s">
         <v>171</v>
       </c>
@@ -7577,7 +7580,7 @@
       <c r="D38" s="30"/>
     </row>
     <row r="39" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A39" s="139"/>
+      <c r="A39" s="149"/>
       <c r="B39" s="57" t="s">
         <v>31</v>
       </c>
@@ -7587,7 +7590,7 @@
       <c r="D39" s="30"/>
     </row>
     <row r="40" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="139"/>
+      <c r="A40" s="149"/>
       <c r="B40" s="57" t="s">
         <v>99</v>
       </c>
@@ -7597,7 +7600,7 @@
       <c r="D40" s="30"/>
     </row>
     <row r="41" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="139"/>
+      <c r="A41" s="149"/>
       <c r="B41" s="57" t="s">
         <v>54</v>
       </c>
@@ -7607,7 +7610,7 @@
       <c r="D41" s="30"/>
     </row>
     <row r="42" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A42" s="139"/>
+      <c r="A42" s="149"/>
       <c r="B42" s="57" t="s">
         <v>57</v>
       </c>
@@ -7617,7 +7620,7 @@
       <c r="D42" s="30"/>
     </row>
     <row r="43" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="139"/>
+      <c r="A43" s="149"/>
       <c r="B43" s="57" t="s">
         <v>40</v>
       </c>
@@ -7627,7 +7630,7 @@
       <c r="D43" s="30"/>
     </row>
     <row r="44" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A44" s="139"/>
+      <c r="A44" s="149"/>
       <c r="B44" s="57" t="s">
         <v>78</v>
       </c>
@@ -7637,7 +7640,7 @@
       <c r="D44" s="30"/>
     </row>
     <row r="45" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A45" s="139"/>
+      <c r="A45" s="149"/>
       <c r="B45" s="57" t="s">
         <v>61</v>
       </c>
@@ -7647,7 +7650,7 @@
       <c r="D45" s="30"/>
     </row>
     <row r="46" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A46" s="139"/>
+      <c r="A46" s="149"/>
       <c r="B46" s="57" t="s">
         <v>97</v>
       </c>
@@ -7657,7 +7660,7 @@
       <c r="D46" s="30"/>
     </row>
     <row r="47" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A47" s="153" t="s">
+      <c r="A47" s="152" t="s">
         <v>243</v>
       </c>
       <c r="B47" s="31" t="s">
@@ -7669,7 +7672,7 @@
       <c r="D47" s="31"/>
     </row>
     <row r="48" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A48" s="153"/>
+      <c r="A48" s="152"/>
       <c r="B48" s="31" t="s">
         <v>77</v>
       </c>
@@ -7679,7 +7682,7 @@
       <c r="D48" s="31"/>
     </row>
     <row r="49" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A49" s="153"/>
+      <c r="A49" s="152"/>
       <c r="B49" s="31" t="s">
         <v>52</v>
       </c>
@@ -7689,7 +7692,7 @@
       <c r="D49" s="31"/>
     </row>
     <row r="50" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A50" s="153"/>
+      <c r="A50" s="152"/>
       <c r="B50" s="31" t="s">
         <v>45</v>
       </c>
@@ -7699,7 +7702,7 @@
       <c r="D50" s="31"/>
     </row>
     <row r="51" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A51" s="153"/>
+      <c r="A51" s="152"/>
       <c r="B51" s="31" t="s">
         <v>87</v>
       </c>
@@ -7709,7 +7712,7 @@
       <c r="D51" s="31"/>
     </row>
     <row r="52" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A52" s="153"/>
+      <c r="A52" s="152"/>
       <c r="B52" s="31" t="s">
         <v>39</v>
       </c>
@@ -7719,7 +7722,7 @@
       <c r="D52" s="31"/>
     </row>
     <row r="53" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A53" s="153"/>
+      <c r="A53" s="152"/>
       <c r="B53" s="31" t="s">
         <v>67</v>
       </c>
@@ -7729,7 +7732,7 @@
       <c r="D53" s="31"/>
     </row>
     <row r="54" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A54" s="153"/>
+      <c r="A54" s="152"/>
       <c r="B54" s="31" t="s">
         <v>48</v>
       </c>
@@ -7739,7 +7742,7 @@
       <c r="D54" s="31"/>
     </row>
     <row r="55" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A55" s="153"/>
+      <c r="A55" s="152"/>
       <c r="B55" s="31" t="s">
         <v>69</v>
       </c>
@@ -7749,7 +7752,7 @@
       <c r="D55" s="31"/>
     </row>
     <row r="56" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A56" s="153"/>
+      <c r="A56" s="152"/>
       <c r="B56" s="31" t="s">
         <v>58</v>
       </c>
@@ -7759,7 +7762,7 @@
       <c r="D56" s="31"/>
     </row>
     <row r="57" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A57" s="153"/>
+      <c r="A57" s="152"/>
       <c r="B57" s="31" t="s">
         <v>101</v>
       </c>
@@ -7769,7 +7772,7 @@
       <c r="D57" s="31"/>
     </row>
     <row r="58" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A58" s="153"/>
+      <c r="A58" s="152"/>
       <c r="B58" s="31" t="s">
         <v>82</v>
       </c>
@@ -7781,7 +7784,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A59" s="153"/>
+      <c r="A59" s="152"/>
       <c r="B59" s="31" t="s">
         <v>47</v>
       </c>
@@ -7791,7 +7794,7 @@
       <c r="D59" s="31"/>
     </row>
     <row r="60" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A60" s="153"/>
+      <c r="A60" s="152"/>
       <c r="B60" s="31" t="s">
         <v>33</v>
       </c>
@@ -7801,7 +7804,7 @@
       <c r="D60" s="31"/>
     </row>
     <row r="61" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A61" s="153"/>
+      <c r="A61" s="152"/>
       <c r="B61" s="31" t="s">
         <v>80</v>
       </c>
@@ -7811,7 +7814,7 @@
       <c r="D61" s="31"/>
     </row>
     <row r="62" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A62" s="153"/>
+      <c r="A62" s="152"/>
       <c r="B62" s="31" t="s">
         <v>37</v>
       </c>
@@ -7821,7 +7824,7 @@
       <c r="D62" s="31"/>
     </row>
     <row r="63" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A63" s="153"/>
+      <c r="A63" s="152"/>
       <c r="B63" s="86" t="s">
         <v>96</v>
       </c>
@@ -7831,7 +7834,7 @@
       <c r="D63" s="31"/>
     </row>
     <row r="64" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A64" s="160" t="s">
+      <c r="A64" s="159" t="s">
         <v>60</v>
       </c>
       <c r="B64" s="76" t="s">
@@ -7843,7 +7846,7 @@
       <c r="D64" s="85"/>
     </row>
     <row r="65" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A65" s="160"/>
+      <c r="A65" s="159"/>
       <c r="B65" s="76" t="s">
         <v>91</v>
       </c>
@@ -7853,7 +7856,7 @@
       <c r="D65" s="85"/>
     </row>
     <row r="66" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A66" s="160"/>
+      <c r="A66" s="159"/>
       <c r="B66" s="76" t="s">
         <v>76</v>
       </c>
@@ -7863,7 +7866,7 @@
       <c r="D66" s="85"/>
     </row>
     <row r="67" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A67" s="161"/>
+      <c r="A67" s="160"/>
       <c r="B67" s="87" t="s">
         <v>175</v>
       </c>
@@ -7873,7 +7876,7 @@
       <c r="D67" s="30"/>
     </row>
     <row r="68" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A68" s="140" t="s">
+      <c r="A68" s="151" t="s">
         <v>34</v>
       </c>
       <c r="B68" s="31" t="s">
@@ -7885,7 +7888,7 @@
       <c r="D68" s="31"/>
     </row>
     <row r="69" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A69" s="140"/>
+      <c r="A69" s="151"/>
       <c r="B69" s="31" t="s">
         <v>44</v>
       </c>
@@ -7895,7 +7898,7 @@
       <c r="D69" s="31"/>
     </row>
     <row r="70" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A70" s="144" t="s">
+      <c r="A70" s="139" t="s">
         <v>63</v>
       </c>
       <c r="B70" s="30" t="s">
@@ -7907,7 +7910,7 @@
       <c r="D70" s="30"/>
     </row>
     <row r="71" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A71" s="145"/>
+      <c r="A71" s="140"/>
       <c r="B71" s="30" t="s">
         <v>176</v>
       </c>
@@ -7929,7 +7932,7 @@
       <c r="D72" s="31"/>
     </row>
     <row r="73" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A73" s="143"/>
+      <c r="A73" s="142"/>
       <c r="B73" s="100" t="s">
         <v>519</v>
       </c>
@@ -7939,7 +7942,7 @@
       <c r="D73" s="100"/>
     </row>
     <row r="74" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A74" s="146" t="s">
+      <c r="A74" s="143" t="s">
         <v>514</v>
       </c>
       <c r="B74" s="87" t="s">
@@ -7951,7 +7954,7 @@
       <c r="D74" s="87"/>
     </row>
     <row r="75" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A75" s="147"/>
+      <c r="A75" s="144"/>
       <c r="B75" s="87" t="s">
         <v>521</v>
       </c>
@@ -7961,7 +7964,7 @@
       <c r="D75" s="87"/>
     </row>
     <row r="76" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A76" s="147"/>
+      <c r="A76" s="144"/>
       <c r="B76" s="87" t="s">
         <v>522</v>
       </c>
@@ -7971,7 +7974,7 @@
       <c r="D76" s="87"/>
     </row>
     <row r="77" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A77" s="145"/>
+      <c r="A77" s="140"/>
       <c r="B77" s="30" t="s">
         <v>523</v>
       </c>
@@ -7993,7 +7996,7 @@
       <c r="D78" s="31"/>
     </row>
     <row r="79" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A79" s="142"/>
+      <c r="A79" s="161"/>
       <c r="B79" s="86" t="s">
         <v>525</v>
       </c>
@@ -8003,7 +8006,7 @@
       <c r="D79" s="86"/>
     </row>
     <row r="80" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A80" s="142"/>
+      <c r="A80" s="161"/>
       <c r="B80" s="86" t="s">
         <v>526</v>
       </c>
@@ -8013,7 +8016,7 @@
       <c r="D80" s="86"/>
     </row>
     <row r="81" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A81" s="142"/>
+      <c r="A81" s="161"/>
       <c r="B81" s="86" t="s">
         <v>527</v>
       </c>
@@ -8023,7 +8026,7 @@
       <c r="D81" s="86"/>
     </row>
     <row r="82" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A82" s="142"/>
+      <c r="A82" s="161"/>
       <c r="B82" s="86" t="s">
         <v>528</v>
       </c>
@@ -8033,7 +8036,7 @@
       <c r="D82" s="86"/>
     </row>
     <row r="83" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A83" s="142"/>
+      <c r="A83" s="161"/>
       <c r="B83" s="86" t="s">
         <v>529</v>
       </c>
@@ -8043,7 +8046,7 @@
       <c r="D83" s="86"/>
     </row>
     <row r="84" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A84" s="143"/>
+      <c r="A84" s="142"/>
       <c r="B84" s="100" t="s">
         <v>530</v>
       </c>
@@ -8053,21 +8056,21 @@
       <c r="D84" s="100"/>
     </row>
     <row r="85" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="154" t="s">
+      <c r="A85" s="153" t="s">
         <v>241</v>
       </c>
-      <c r="B85" s="155"/>
-      <c r="C85" s="155"/>
-      <c r="D85" s="156"/>
+      <c r="B85" s="154"/>
+      <c r="C85" s="154"/>
+      <c r="D85" s="155"/>
     </row>
     <row r="86" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="157"/>
-      <c r="B86" s="158"/>
-      <c r="C86" s="158"/>
-      <c r="D86" s="159"/>
+      <c r="A86" s="156"/>
+      <c r="B86" s="157"/>
+      <c r="C86" s="157"/>
+      <c r="D86" s="158"/>
     </row>
     <row r="87" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="139" t="s">
+      <c r="A87" s="149" t="s">
         <v>244</v>
       </c>
       <c r="B87" s="57" t="s">
@@ -8079,7 +8082,7 @@
       <c r="D87" s="30"/>
     </row>
     <row r="88" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="139"/>
+      <c r="A88" s="149"/>
       <c r="B88" s="57" t="s">
         <v>38</v>
       </c>
@@ -8089,7 +8092,7 @@
       <c r="D88" s="30"/>
     </row>
     <row r="89" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="139"/>
+      <c r="A89" s="149"/>
       <c r="B89" s="57" t="s">
         <v>95</v>
       </c>
@@ -8099,7 +8102,7 @@
       <c r="D89" s="30"/>
     </row>
     <row r="90" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="139"/>
+      <c r="A90" s="149"/>
       <c r="B90" s="57" t="s">
         <v>81</v>
       </c>
@@ -8109,7 +8112,7 @@
       <c r="D90" s="30"/>
     </row>
     <row r="91" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="139"/>
+      <c r="A91" s="149"/>
       <c r="B91" s="57" t="s">
         <v>32</v>
       </c>
@@ -8119,7 +8122,7 @@
       <c r="D91" s="30"/>
     </row>
     <row r="92" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="139"/>
+      <c r="A92" s="149"/>
       <c r="B92" s="57" t="s">
         <v>55</v>
       </c>
@@ -8129,7 +8132,7 @@
       <c r="D92" s="30"/>
     </row>
     <row r="93" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="139"/>
+      <c r="A93" s="149"/>
       <c r="B93" s="57" t="s">
         <v>73</v>
       </c>
@@ -8139,7 +8142,7 @@
       <c r="D93" s="30"/>
     </row>
     <row r="94" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="139"/>
+      <c r="A94" s="149"/>
       <c r="B94" s="57" t="s">
         <v>100</v>
       </c>
@@ -8149,7 +8152,7 @@
       <c r="D94" s="30"/>
     </row>
     <row r="95" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A95" s="139"/>
+      <c r="A95" s="149"/>
       <c r="B95" s="57" t="s">
         <v>184</v>
       </c>
@@ -8159,7 +8162,7 @@
       <c r="D95" s="30"/>
     </row>
     <row r="96" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A96" s="139"/>
+      <c r="A96" s="149"/>
       <c r="B96" s="57" t="s">
         <v>666</v>
       </c>
@@ -8169,7 +8172,7 @@
       <c r="D96" s="30"/>
     </row>
     <row r="97" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A97" s="153" t="s">
+      <c r="A97" s="152" t="s">
         <v>253</v>
       </c>
       <c r="B97" s="31" t="s">
@@ -8181,7 +8184,7 @@
       <c r="D97" s="31"/>
     </row>
     <row r="98" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A98" s="153"/>
+      <c r="A98" s="152"/>
       <c r="B98" s="31" t="s">
         <v>187</v>
       </c>
@@ -8191,7 +8194,7 @@
       <c r="D98" s="31"/>
     </row>
     <row r="99" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A99" s="153"/>
+      <c r="A99" s="152"/>
       <c r="B99" s="31" t="s">
         <v>189</v>
       </c>
@@ -8201,21 +8204,21 @@
       <c r="D99" s="31"/>
     </row>
     <row r="100" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="154" t="s">
+      <c r="A100" s="153" t="s">
         <v>123</v>
       </c>
-      <c r="B100" s="155"/>
-      <c r="C100" s="155"/>
-      <c r="D100" s="156"/>
+      <c r="B100" s="154"/>
+      <c r="C100" s="154"/>
+      <c r="D100" s="155"/>
     </row>
     <row r="101" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="157"/>
-      <c r="B101" s="158"/>
-      <c r="C101" s="158"/>
-      <c r="D101" s="159"/>
+      <c r="A101" s="156"/>
+      <c r="B101" s="157"/>
+      <c r="C101" s="157"/>
+      <c r="D101" s="158"/>
     </row>
     <row r="102" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A102" s="139" t="s">
+      <c r="A102" s="149" t="s">
         <v>245</v>
       </c>
       <c r="B102" s="57" t="s">
@@ -8227,7 +8230,7 @@
       <c r="D102" s="30"/>
     </row>
     <row r="103" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A103" s="139"/>
+      <c r="A103" s="149"/>
       <c r="B103" s="57" t="s">
         <v>53</v>
       </c>
@@ -8237,7 +8240,7 @@
       <c r="D103" s="30"/>
     </row>
     <row r="104" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A104" s="139"/>
+      <c r="A104" s="149"/>
       <c r="B104" s="57" t="s">
         <v>191</v>
       </c>
@@ -8247,7 +8250,7 @@
       <c r="D104" s="30"/>
     </row>
     <row r="105" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A105" s="139"/>
+      <c r="A105" s="149"/>
       <c r="B105" s="57" t="s">
         <v>559</v>
       </c>
@@ -8257,7 +8260,7 @@
       <c r="D105" s="30"/>
     </row>
     <row r="106" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A106" s="139"/>
+      <c r="A106" s="149"/>
       <c r="B106" s="57" t="s">
         <v>192</v>
       </c>
@@ -8267,7 +8270,7 @@
       <c r="D106" s="30"/>
     </row>
     <row r="107" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A107" s="139"/>
+      <c r="A107" s="149"/>
       <c r="B107" s="57" t="s">
         <v>194</v>
       </c>
@@ -8277,7 +8280,7 @@
       <c r="D107" s="30"/>
     </row>
     <row r="108" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A108" s="139"/>
+      <c r="A108" s="149"/>
       <c r="B108" s="57" t="s">
         <v>195</v>
       </c>
@@ -8287,7 +8290,7 @@
       <c r="D108" s="30"/>
     </row>
     <row r="109" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A109" s="139"/>
+      <c r="A109" s="149"/>
       <c r="B109" s="57" t="s">
         <v>197</v>
       </c>
@@ -8297,7 +8300,7 @@
       <c r="D109" s="30"/>
     </row>
     <row r="110" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A110" s="139"/>
+      <c r="A110" s="149"/>
       <c r="B110" s="57" t="s">
         <v>563</v>
       </c>
@@ -8307,7 +8310,7 @@
       <c r="D110" s="30"/>
     </row>
     <row r="111" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A111" s="139"/>
+      <c r="A111" s="149"/>
       <c r="B111" s="57" t="s">
         <v>79</v>
       </c>
@@ -8317,7 +8320,7 @@
       <c r="D111" s="30"/>
     </row>
     <row r="112" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A112" s="139"/>
+      <c r="A112" s="149"/>
       <c r="B112" s="57" t="s">
         <v>85</v>
       </c>
@@ -8327,7 +8330,7 @@
       <c r="D112" s="30"/>
     </row>
     <row r="113" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A113" s="152"/>
+      <c r="A113" s="150"/>
       <c r="B113" s="57" t="s">
         <v>94</v>
       </c>
@@ -8337,7 +8340,7 @@
       <c r="D113" s="30"/>
     </row>
     <row r="114" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="148" t="s">
+      <c r="A114" s="145" t="s">
         <v>246</v>
       </c>
       <c r="B114" s="101" t="s">
@@ -8349,7 +8352,7 @@
       <c r="D114" s="31"/>
     </row>
     <row r="115" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A115" s="148"/>
+      <c r="A115" s="145"/>
       <c r="B115" s="101" t="s">
         <v>201</v>
       </c>
@@ -8359,7 +8362,7 @@
       <c r="D115" s="31"/>
     </row>
     <row r="116" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A116" s="148"/>
+      <c r="A116" s="145"/>
       <c r="B116" s="101" t="s">
         <v>202</v>
       </c>
@@ -8369,7 +8372,7 @@
       <c r="D116" s="31"/>
     </row>
     <row r="117" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A117" s="148"/>
+      <c r="A117" s="145"/>
       <c r="B117" s="101" t="s">
         <v>457</v>
       </c>
@@ -8379,7 +8382,7 @@
       <c r="D117" s="31"/>
     </row>
     <row r="118" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A118" s="148"/>
+      <c r="A118" s="145"/>
       <c r="B118" s="101" t="s">
         <v>203</v>
       </c>
@@ -8389,7 +8392,7 @@
       <c r="D118" s="31"/>
     </row>
     <row r="119" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A119" s="148"/>
+      <c r="A119" s="145"/>
       <c r="B119" s="101" t="s">
         <v>204</v>
       </c>
@@ -8399,7 +8402,7 @@
       <c r="D119" s="31"/>
     </row>
     <row r="120" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A120" s="148"/>
+      <c r="A120" s="145"/>
       <c r="B120" s="101" t="s">
         <v>205</v>
       </c>
@@ -8409,7 +8412,7 @@
       <c r="D120" s="31"/>
     </row>
     <row r="121" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A121" s="148"/>
+      <c r="A121" s="145"/>
       <c r="B121" s="101" t="s">
         <v>206</v>
       </c>
@@ -8419,7 +8422,7 @@
       <c r="D121" s="31"/>
     </row>
     <row r="122" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A122" s="148"/>
+      <c r="A122" s="145"/>
       <c r="B122" s="101" t="s">
         <v>208</v>
       </c>
@@ -8429,7 +8432,7 @@
       <c r="D122" s="31"/>
     </row>
     <row r="123" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A123" s="148"/>
+      <c r="A123" s="145"/>
       <c r="B123" s="101" t="s">
         <v>209</v>
       </c>
@@ -8439,7 +8442,7 @@
       <c r="D123" s="31"/>
     </row>
     <row r="124" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A124" s="148"/>
+      <c r="A124" s="145"/>
       <c r="B124" s="101" t="s">
         <v>212</v>
       </c>
@@ -8449,7 +8452,7 @@
       <c r="D124" s="31"/>
     </row>
     <row r="125" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A125" s="148"/>
+      <c r="A125" s="145"/>
       <c r="B125" s="101" t="s">
         <v>214</v>
       </c>
@@ -8459,7 +8462,7 @@
       <c r="D125" s="31"/>
     </row>
     <row r="126" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A126" s="148"/>
+      <c r="A126" s="145"/>
       <c r="B126" s="102" t="s">
         <v>216</v>
       </c>
@@ -8469,7 +8472,7 @@
       <c r="D126" s="31"/>
     </row>
     <row r="127" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A127" s="148"/>
+      <c r="A127" s="145"/>
       <c r="B127" s="78" t="s">
         <v>458</v>
       </c>
@@ -8479,7 +8482,7 @@
       <c r="D127" s="31"/>
     </row>
     <row r="128" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A128" s="148"/>
+      <c r="A128" s="145"/>
       <c r="B128" s="78" t="s">
         <v>569</v>
       </c>
@@ -8489,7 +8492,7 @@
       <c r="D128" s="31"/>
     </row>
     <row r="129" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A129" s="148"/>
+      <c r="A129" s="145"/>
       <c r="B129" s="118" t="s">
         <v>556</v>
       </c>
@@ -8499,7 +8502,7 @@
       <c r="D129" s="31"/>
     </row>
     <row r="130" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A130" s="148"/>
+      <c r="A130" s="145"/>
       <c r="B130" s="101" t="s">
         <v>210</v>
       </c>
@@ -8509,7 +8512,7 @@
       <c r="D130" s="31"/>
     </row>
     <row r="131" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A131" s="148"/>
+      <c r="A131" s="145"/>
       <c r="B131" s="101" t="s">
         <v>218</v>
       </c>
@@ -8519,7 +8522,7 @@
       <c r="D131" s="31"/>
     </row>
     <row r="132" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A132" s="148"/>
+      <c r="A132" s="145"/>
       <c r="B132" s="101" t="s">
         <v>220</v>
       </c>
@@ -8529,7 +8532,7 @@
       <c r="D132" s="31"/>
     </row>
     <row r="133" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A133" s="148"/>
+      <c r="A133" s="145"/>
       <c r="B133" s="101" t="s">
         <v>222</v>
       </c>
@@ -8539,7 +8542,7 @@
       <c r="D133" s="31"/>
     </row>
     <row r="134" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A134" s="148"/>
+      <c r="A134" s="145"/>
       <c r="B134" s="101" t="s">
         <v>66</v>
       </c>
@@ -8549,7 +8552,7 @@
       <c r="D134" s="31"/>
     </row>
     <row r="135" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A135" s="148"/>
+      <c r="A135" s="145"/>
       <c r="B135" s="101" t="s">
         <v>225</v>
       </c>
@@ -8559,7 +8562,7 @@
       <c r="D135" s="31"/>
     </row>
     <row r="136" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A136" s="148"/>
+      <c r="A136" s="145"/>
       <c r="B136" s="101" t="s">
         <v>561</v>
       </c>
@@ -8569,7 +8572,7 @@
       <c r="D136" s="31"/>
     </row>
     <row r="137" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A137" s="148"/>
+      <c r="A137" s="145"/>
       <c r="B137" s="101" t="s">
         <v>227</v>
       </c>
@@ -8579,7 +8582,7 @@
       <c r="D137" s="31"/>
     </row>
     <row r="138" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A138" s="148"/>
+      <c r="A138" s="145"/>
       <c r="B138" s="101" t="s">
         <v>567</v>
       </c>
@@ -8589,7 +8592,7 @@
       <c r="D138" s="31"/>
     </row>
     <row r="139" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A139" s="148"/>
+      <c r="A139" s="145"/>
       <c r="B139" s="101" t="s">
         <v>228</v>
       </c>
@@ -8599,7 +8602,7 @@
       <c r="D139" s="31"/>
     </row>
     <row r="140" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A140" s="148"/>
+      <c r="A140" s="145"/>
       <c r="B140" s="101" t="s">
         <v>230</v>
       </c>
@@ -8609,7 +8612,7 @@
       <c r="D140" s="31"/>
     </row>
     <row r="141" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A141" s="148"/>
+      <c r="A141" s="145"/>
       <c r="B141" s="101" t="s">
         <v>232</v>
       </c>
@@ -8619,7 +8622,7 @@
       <c r="D141" s="31"/>
     </row>
     <row r="142" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A142" s="148"/>
+      <c r="A142" s="145"/>
       <c r="B142" s="101" t="s">
         <v>233</v>
       </c>
@@ -8629,7 +8632,7 @@
       <c r="D142" s="31"/>
     </row>
     <row r="143" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A143" s="148"/>
+      <c r="A143" s="145"/>
       <c r="B143" s="101" t="s">
         <v>235</v>
       </c>
@@ -8639,7 +8642,7 @@
       <c r="D143" s="31"/>
     </row>
     <row r="144" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A144" s="148"/>
+      <c r="A144" s="145"/>
       <c r="B144" s="101" t="s">
         <v>565</v>
       </c>
@@ -8649,7 +8652,7 @@
       <c r="D144" s="31"/>
     </row>
     <row r="145" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A145" s="148"/>
+      <c r="A145" s="145"/>
       <c r="B145" s="101" t="s">
         <v>236</v>
       </c>
@@ -8659,7 +8662,7 @@
       <c r="D145" s="31"/>
     </row>
     <row r="146" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A146" s="148"/>
+      <c r="A146" s="145"/>
       <c r="B146" s="101" t="s">
         <v>238</v>
       </c>
@@ -8669,7 +8672,7 @@
       <c r="D146" s="31"/>
     </row>
     <row r="147" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A147" s="148"/>
+      <c r="A147" s="145"/>
       <c r="B147" s="101" t="s">
         <v>247</v>
       </c>
@@ -8679,7 +8682,7 @@
       <c r="D147" s="31"/>
     </row>
     <row r="148" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A148" s="148"/>
+      <c r="A148" s="145"/>
       <c r="B148" s="101" t="s">
         <v>239</v>
       </c>
@@ -8689,7 +8692,7 @@
       <c r="D148" s="31"/>
     </row>
     <row r="149" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A149" s="148"/>
+      <c r="A149" s="145"/>
       <c r="B149" s="101" t="s">
         <v>98</v>
       </c>
@@ -8706,6 +8709,12 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A15:A32"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A78:A84"/>
+    <mergeCell ref="A70:A71"/>
+    <mergeCell ref="A72:A73"/>
+    <mergeCell ref="A74:A77"/>
     <mergeCell ref="A114:A149"/>
     <mergeCell ref="A1:D7"/>
     <mergeCell ref="A8:D10"/>
@@ -8719,12 +8728,6 @@
     <mergeCell ref="A64:A67"/>
     <mergeCell ref="A47:A63"/>
     <mergeCell ref="A35:A46"/>
-    <mergeCell ref="A15:A32"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A78:A84"/>
-    <mergeCell ref="A70:A71"/>
-    <mergeCell ref="A72:A73"/>
-    <mergeCell ref="A74:A77"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -9304,66 +9307,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="149"/>
-      <c r="B1" s="149"/>
-      <c r="C1" s="149"/>
-      <c r="D1" s="149"/>
+      <c r="A1" s="146"/>
+      <c r="B1" s="146"/>
+      <c r="C1" s="146"/>
+      <c r="D1" s="146"/>
     </row>
     <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="149"/>
-      <c r="B2" s="149"/>
-      <c r="C2" s="149"/>
-      <c r="D2" s="149"/>
+      <c r="A2" s="146"/>
+      <c r="B2" s="146"/>
+      <c r="C2" s="146"/>
+      <c r="D2" s="146"/>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="149"/>
-      <c r="B3" s="149"/>
-      <c r="C3" s="149"/>
-      <c r="D3" s="149"/>
+      <c r="A3" s="146"/>
+      <c r="B3" s="146"/>
+      <c r="C3" s="146"/>
+      <c r="D3" s="146"/>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="149"/>
-      <c r="B4" s="149"/>
-      <c r="C4" s="149"/>
-      <c r="D4" s="149"/>
+      <c r="A4" s="146"/>
+      <c r="B4" s="146"/>
+      <c r="C4" s="146"/>
+      <c r="D4" s="146"/>
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="149"/>
-      <c r="B5" s="149"/>
-      <c r="C5" s="149"/>
-      <c r="D5" s="149"/>
+      <c r="A5" s="146"/>
+      <c r="B5" s="146"/>
+      <c r="C5" s="146"/>
+      <c r="D5" s="146"/>
     </row>
     <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="149"/>
-      <c r="B6" s="149"/>
-      <c r="C6" s="149"/>
-      <c r="D6" s="149"/>
+      <c r="A6" s="146"/>
+      <c r="B6" s="146"/>
+      <c r="C6" s="146"/>
+      <c r="D6" s="146"/>
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="149"/>
-      <c r="B7" s="149"/>
-      <c r="C7" s="149"/>
-      <c r="D7" s="149"/>
+      <c r="A7" s="146"/>
+      <c r="B7" s="146"/>
+      <c r="C7" s="146"/>
+      <c r="D7" s="146"/>
     </row>
     <row r="8" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="150" t="s">
+      <c r="A8" s="147" t="s">
         <v>415</v>
       </c>
-      <c r="B8" s="150"/>
-      <c r="C8" s="150"/>
-      <c r="D8" s="150"/>
+      <c r="B8" s="147"/>
+      <c r="C8" s="147"/>
+      <c r="D8" s="147"/>
     </row>
     <row r="9" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="150"/>
-      <c r="B9" s="150"/>
-      <c r="C9" s="150"/>
-      <c r="D9" s="150"/>
+      <c r="A9" s="147"/>
+      <c r="B9" s="147"/>
+      <c r="C9" s="147"/>
+      <c r="D9" s="147"/>
     </row>
     <row r="10" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="151"/>
-      <c r="B10" s="151"/>
-      <c r="C10" s="151"/>
-      <c r="D10" s="151"/>
+      <c r="A10" s="148"/>
+      <c r="B10" s="148"/>
+      <c r="C10" s="148"/>
+      <c r="D10" s="148"/>
     </row>
     <row r="11" spans="1:4" s="2" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="32" t="s">
@@ -9392,12 +9395,12 @@
       <c r="D12" s="32"/>
     </row>
     <row r="13" spans="1:4" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="154" t="s">
+      <c r="A13" s="153" t="s">
         <v>416</v>
       </c>
-      <c r="B13" s="155"/>
-      <c r="C13" s="155"/>
-      <c r="D13" s="156"/>
+      <c r="B13" s="154"/>
+      <c r="C13" s="154"/>
+      <c r="D13" s="155"/>
     </row>
     <row r="14" spans="1:4" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="171"/>
@@ -9745,8 +9748,8 @@
   </sheetPr>
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9817,7 +9820,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="130" t="s">
-        <v>364</v>
+        <v>672</v>
       </c>
       <c r="B8" s="130"/>
       <c r="C8" s="130"/>

</xml_diff>